<commit_message>
build blogs excel update
</commit_message>
<xml_diff>
--- a/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Build - 5840900.xlsx
+++ b/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Build - 5840900.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DD56AE-F8C9-4D67-B348-80A92366C9AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E88F2-1A3D-42D3-815E-EEAEC6B1FDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3675" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2010" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,6 +432,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,16 +454,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -796,7 +800,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,40 +813,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -880,13 +884,13 @@
       <c r="B6" s="2">
         <v>88</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F6" t="b">
@@ -909,7 +913,7 @@
       <c r="B7" s="3">
         <v>92</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="13" t="s">
@@ -990,19 +994,19 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="6">
         <v>63</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F10" t="b">
@@ -1019,19 +1023,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="6">
         <v>76</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="b">
@@ -1045,13 +1049,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>83</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -1083,6 +1087,7 @@
       <c r="E13" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="F13" s="23"/>
       <c r="G13" t="b">
         <v>1</v>
       </c>
@@ -1100,15 +1105,16 @@
       <c r="B14" s="2">
         <v>93</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="17" t="s">
         <v>30</v>
       </c>
+      <c r="F14" s="23"/>
       <c r="G14" t="b">
         <v>1</v>
       </c>
@@ -1117,7 +1123,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6">
@@ -1126,13 +1132,16 @@
       <c r="C15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="H15" t="b">
@@ -1218,20 +1227,23 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="6">
         <v>87</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="17" t="s">
         <v>30</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
@@ -1267,20 +1279,23 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="6">
         <v>68</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="17" t="s">
         <v>30</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1425,40 +1440,40 @@
       <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1957,9 +1972,20 @@
     <hyperlink ref="C12" r:id="rId12" xr:uid="{873FB4BE-52F6-499B-8C42-5C570512CE0E}"/>
     <hyperlink ref="C14" r:id="rId13" xr:uid="{978C4615-2F9D-4889-B48A-A511C0E0EC45}"/>
     <hyperlink ref="E14" r:id="rId14" xr:uid="{DA00450B-8B9E-40B7-BE1C-64A896250774}"/>
+    <hyperlink ref="A12" r:id="rId15" xr:uid="{17275F18-93E0-4440-BD22-F931CC213D33}"/>
+    <hyperlink ref="D15" r:id="rId16" xr:uid="{002CAA8A-9A91-40B0-93D9-5DBCEE976EC5}"/>
+    <hyperlink ref="A15" r:id="rId17" xr:uid="{C38D8D58-D57A-4CFB-8131-CEC824506DF2}"/>
+    <hyperlink ref="E15" r:id="rId18" xr:uid="{0F38F8D5-BF9D-4A02-A1E0-6CE39B03D642}"/>
+    <hyperlink ref="A19" r:id="rId19" xr:uid="{31D26307-4EBB-49F9-A8F1-8E3060090CB8}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{4178E223-B0FE-4009-914A-88048ADFE092}"/>
+    <hyperlink ref="D19" r:id="rId21" xr:uid="{9B33C9DB-71A4-4AAC-A576-2B28F431DAD4}"/>
+    <hyperlink ref="E19" r:id="rId22" xr:uid="{1B3DCB10-DD23-4E27-81AA-1199513CF636}"/>
+    <hyperlink ref="C21" r:id="rId23" xr:uid="{1069B70A-DAFE-4823-B1D1-F44757447DC3}"/>
+    <hyperlink ref="A21" r:id="rId24" xr:uid="{0AA6412C-1CBA-416E-B3C6-AD8F6DFCF146}"/>
+    <hyperlink ref="E21" r:id="rId25" xr:uid="{0065E1E8-4DEA-4DD1-86A0-2E8C8CCD0F14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>